<commit_message>
Update Data by bot, scripted by HH
</commit_message>
<xml_diff>
--- a/业绩报表/003028.xlsx
+++ b/业绩报表/003028.xlsx
@@ -1024,38 +1024,26 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2020-09-30 00:00:00</t>
+          <t>2019-09-30 00:00:00</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1.52</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1.46</v>
-      </c>
+        <v>0.97</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
       <c r="K5" t="n">
-        <v>664959193.23</v>
+        <v>509598813.87</v>
       </c>
       <c r="L5" t="n">
-        <v>124771015.43</v>
-      </c>
-      <c r="M5" t="n">
-        <v>30.31</v>
-      </c>
-      <c r="N5" t="n">
-        <v>30.4868016038</v>
-      </c>
-      <c r="O5" t="n">
-        <v>57.0334171895</v>
-      </c>
-      <c r="P5" t="n">
-        <v>5.201814431387</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.404062484307</v>
-      </c>
+        <v>79455072.47</v>
+      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
       <c r="R5" t="n">
-        <v>30.5668683581</v>
+        <v>27.0353207426</v>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
@@ -1084,22 +1072,22 @@
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>2020Q3</t>
+          <t>2019Q3</t>
         </is>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>2020年 三季报</t>
+          <t>2019年 三季报</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">

</xml_diff>